<commit_message>
Fixed an issue where out of range levels generate invalid images Various bugfixes Removed various redundant codes
</commit_message>
<xml_diff>
--- a/asset/rush_duel_card_maker_batch_template_0.01.xlsx
+++ b/asset/rush_duel_card_maker_batch_template_0.01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Rush Duel Card Maker\asset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81277143-B853-4111-AFB6-992B2694C11E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D53299B-2CB0-4D18-8254-F7CF03BC5302}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3AA2F37B-73A0-42DF-90DC-52C5D1F12CE9}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="46">
   <si>
     <t>Set No.</t>
   </si>
@@ -166,16 +166,13 @@
     <t>01010103</t>
   </si>
   <si>
-    <t>Custom Card!!</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
     <t>&lt;b&gt;[REQUIREMENT]:&lt;/b&gt;&lt;br&gt; None&lt;br&gt;&lt;b&gt;[CONTINUOUS EFFECT]:&lt;/b&gt;&lt;br&gt;You can use custom cards in duels.</t>
   </si>
   <si>
     <t>https://i.ibb.co/NncgcGk/214f381b564cbf8f08da0b5fa18e8b63.png</t>
+  </si>
+  <si>
+    <t>Custom Card!</t>
   </si>
 </sst>
 </file>
@@ -280,8 +277,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{35B671B1-E6FC-4EE9-AE74-3184ADA78415}" name="Table1" displayName="Table1" ref="A1:P17" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:P17" xr:uid="{35B671B1-E6FC-4EE9-AE74-3184ADA78415}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{35B671B1-E6FC-4EE9-AE74-3184ADA78415}" name="Table1" displayName="Table1" ref="A1:P13" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:P13" xr:uid="{35B671B1-E6FC-4EE9-AE74-3184ADA78415}"/>
   <tableColumns count="16">
     <tableColumn id="1" xr3:uid="{1AF4F2AE-61CA-4C17-AD82-6C9753D166FF}" name="Set No." dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{744B3171-45E7-4BB1-B4D4-9B37A744837D}" name="Name"/>
@@ -601,10 +598,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE16C02C-31FC-4184-9EC8-39D03146F180}">
-  <dimension ref="A1:P17"/>
+  <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -681,16 +678,13 @@
         <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="G2" t="s">
         <v>19</v>
@@ -704,20 +698,11 @@
       <c r="J2">
         <v>2000</v>
       </c>
-      <c r="K2" t="b">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2" t="s">
-        <v>35</v>
-      </c>
       <c r="N2" t="s">
         <v>28</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="P2" t="s">
         <v>38</v>
@@ -736,11 +721,8 @@
       <c r="D3" t="b">
         <v>0</v>
       </c>
-      <c r="E3" t="s">
-        <v>34</v>
-      </c>
       <c r="F3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G3" t="s">
         <v>20</v>
@@ -767,10 +749,10 @@
         <v>32</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
@@ -778,7 +760,7 @@
         <v>42</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C4" t="s">
         <v>16</v>
@@ -789,35 +771,11 @@
       <c r="E4" t="s">
         <v>34</v>
       </c>
-      <c r="F4" t="s">
+      <c r="N4" t="s">
+        <v>43</v>
+      </c>
+      <c r="O4" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="G4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4" t="b">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4" t="s">
-        <v>36</v>
-      </c>
-      <c r="N4" t="s">
-        <v>45</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="P4" t="s">
         <v>39</v>
@@ -858,30 +816,11 @@
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="O13" s="3"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A14" s="2"/>
-      <c r="O14" s="3"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A15" s="2"/>
-      <c r="O15" s="3"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A16" s="2"/>
-      <c r="O16" s="3"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A17" s="2"/>
-      <c r="O17" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="A2:A3" numberStoredAsText="1"/>
-  </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
@@ -892,37 +831,37 @@
           <x14:formula1>
             <xm:f>Helper!$A$1:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C17</xm:sqref>
+          <xm:sqref>C2:C13</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{3AC737DD-3BD9-4412-9F63-6F83AEF3B8C5}">
           <x14:formula1>
             <xm:f>Helper!$D$1:$D$2</xm:f>
           </x14:formula1>
-          <xm:sqref>K2:K17 D2:D17</xm:sqref>
+          <xm:sqref>K2:K13 D2:D13</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8E1FE465-5D87-4CF4-8661-128083E422F3}">
           <x14:formula1>
             <xm:f>Helper!$B$1:$B$6</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G17</xm:sqref>
+          <xm:sqref>G2:G13</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{7ECB9960-F7C4-41F0-8227-5078C8D92B74}">
           <x14:formula1>
             <xm:f>Helper!$C$1:$C$12</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:H17</xm:sqref>
+          <xm:sqref>H2:H13</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{20D5C375-4070-4F91-8C28-624365323EFA}">
           <x14:formula1>
             <xm:f>Helper!$E$1:$E$2</xm:f>
           </x14:formula1>
-          <xm:sqref>M2:M17</xm:sqref>
+          <xm:sqref>M2:M13</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{A0E5B3A8-76CA-4C33-8D31-63C5A01100CC}">
           <x14:formula1>
             <xm:f>Helper!$F$1:$F$2</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E17</xm:sqref>
+          <xm:sqref>E2:E13</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>